<commit_message>
GUI: NextAndBackFunctionality - Tagged a test case. Updated statistics.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/AllSteps/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/AllSteps/_Test_Suite_Statistics.xlsx
@@ -158,141 +158,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="180">
-          <stop position="0">
-            <color rgb="FF66FF66"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="180">
-          <stop position="0">
-            <color rgb="FF66FF66"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill>
@@ -802,7 +668,7 @@
   <dimension ref="A1:L175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,7 +773,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>12</v>
@@ -917,7 +783,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C$3:C36)</f>
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -954,86 +820,86 @@
     <sortCondition ref="F2"/>
   </sortState>
   <conditionalFormatting sqref="D4:D50 I2">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="25" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="25" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D1048576 I2 D1">
-    <cfRule type="containsText" dxfId="30" priority="17" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="22" priority="17" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="18" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="21" priority="18" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="19" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="20" priority="19" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="20" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="19" priority="20" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="21" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="18" priority="21" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="22" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="17" priority="22" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="23" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="16" priority="23" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="16" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(D3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="22" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="14" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="13" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="12" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="11" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="10" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="9" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="8" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="13" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="6" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="5" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="4" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="3" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="2" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="1" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="0" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
FUNCTIONALITY: Wrote a new suite.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/AllSteps/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/AllSteps/_Test_Suite_Statistics.xlsx
@@ -48,9 +48,6 @@
     <t>Percentage Automated:</t>
   </si>
   <si>
-    <t>NextAndBackButtons</t>
-  </si>
-  <si>
     <t>NextAndBackFunctionality</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Suited to Manual</t>
+  </si>
+  <si>
+    <t>CancelButton</t>
   </si>
 </sst>
 </file>
@@ -158,7 +158,141 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="40">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill>
+          <stop position="0">
+            <color rgb="FF00B0F0"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="180">
+          <stop position="0">
+            <color rgb="FF66FF66"/>
+          </stop>
+          <stop position="1">
+            <color rgb="FF00B050"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor rgb="FF66FF66"/>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -665,10 +799,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L175"/>
+  <dimension ref="A1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +817,7 @@
     <col min="9" max="9" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -697,105 +831,104 @@
         <v>1</v>
       </c>
       <c r="E1" s="4">
-        <f>COUNTA($A$3:A37)</f>
-        <v>2</v>
+        <f>COUNTA($A:$A)-1</f>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="6">
-        <f>COUNTIF($D$3:D36,"Ready to Write")+COUNTIF($D$3:D36,"Outdated")</f>
-        <v>1</v>
+        <f>COUNTIF($D:$D,"Ready to Write")+COUNTIF($D:$D,"Outdated")</f>
+        <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3">
-        <f>SUM(G1:G2)</f>
-        <v>1</v>
+        <f>SUM(G1:G1)</f>
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="6">
+        <f>COUNTIF($D:$D,"Automated")+COUNTIF($D:$D,"Finished")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>16</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L2" s="6">
-        <f>COUNTIF($D$3:D36,"Automated")+COUNTIF($D$3:D36,"Finished")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="3">
-        <f>SUM($C$3:C36)</f>
-        <v>13</v>
+        <f>SUM($C:$C)</f>
+        <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="F5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="3">
-        <f>SUM($B$3:B36)</f>
+        <f>SUM($B:$B)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F6" s="3" t="s">
         <v>9</v>
       </c>
@@ -804,7 +937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="73" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -816,35 +949,60 @@
     <row r="163" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="175" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState ref="F2:J8">
-    <sortCondition ref="F2"/>
-  </sortState>
-  <conditionalFormatting sqref="D4:D50 I2">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="25" stopIfTrue="1">
-      <formula>LEN(TRIM(D2))&gt;0</formula>
+  <conditionalFormatting sqref="D5:D51">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="33" stopIfTrue="1">
+      <formula>LEN(TRIM(D5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:D1048576 I2 D1">
+  <conditionalFormatting sqref="D5:D1048576 D1">
+    <cfRule type="containsText" dxfId="30" priority="25" stopIfTrue="1" operator="containsText" text="Finished">
+      <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="26" stopIfTrue="1" operator="containsText" text="Automated">
+      <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="27" stopIfTrue="1" operator="containsText" text="Under Review">
+      <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="28" stopIfTrue="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="29" stopIfTrue="1" operator="containsText" text="Writing">
+      <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="25" priority="30" stopIfTrue="1" operator="containsText" text="Ready to Write">
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="31" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="24" stopIfTrue="1">
+      <formula>LEN(TRIM(D4))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4">
     <cfRule type="containsText" dxfId="22" priority="17" stopIfTrue="1" operator="containsText" text="Finished">
-      <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Finished",D4)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="21" priority="18" stopIfTrue="1" operator="containsText" text="Automated">
-      <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Automated",D4)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="20" priority="19" stopIfTrue="1" operator="containsText" text="Under Review">
-      <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Under Review",D4)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="19" priority="20" stopIfTrue="1" operator="containsText" text="Testing">
-      <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Testing",D4)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="18" priority="21" stopIfTrue="1" operator="containsText" text="Writing">
-      <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Writing",D4)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="17" priority="22" stopIfTrue="1" operator="containsText" text="Ready to Write">
-      <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Ready to Write",D4)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="16" priority="23" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
-      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">

</xml_diff>

<commit_message>
FUNCTIONALITY: Tagged a test case that we can't automate.
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Create/AllSteps/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Create/AllSteps/_Test_Suite_Statistics.xlsx
@@ -737,17 +737,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="45.7109375" style="2" customWidth="1"/>
     <col min="2" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="50.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="45.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="7.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="9" max="9" width="3.7109375" customWidth="1"/>
@@ -840,7 +840,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -851,7 +851,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>11</v>
@@ -870,7 +870,7 @@
       </c>
       <c r="G6" s="8">
         <f>G5/G4</f>
-        <v>0.5</v>
+        <v>0.53333333333333333</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>